<commit_message>
[ADD] commit before merge
</commit_message>
<xml_diff>
--- a/data/experimental/Biomass_exp_composition.xlsx
+++ b/data/experimental/Biomass_exp_composition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bisbii\PythonProjects\GSMMutils\data\experimental\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bisbii\PythonProjects\dynamic_model\data\experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A9884-C2B2-4DFF-A7D6-04F2E4B26AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46430A6A-1ABA-4B9E-A8C4-D6DFDB9A2D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="macromolecules" sheetId="1" r:id="rId1"/>
@@ -37,28 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
-  <si>
-    <t>PC1</t>
-  </si>
-  <si>
-    <t>PC2</t>
-  </si>
-  <si>
-    <t>PC3</t>
-  </si>
-  <si>
-    <t>PC4</t>
-  </si>
-  <si>
-    <t>RPC1</t>
-  </si>
-  <si>
-    <t>RPC2</t>
-  </si>
-  <si>
-    <t>RPC3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Protein</t>
   </si>
@@ -130,6 +109,9 @@
   </si>
   <si>
     <t>SC</t>
+  </si>
+  <si>
+    <t>PC</t>
   </si>
 </sst>
 </file>
@@ -457,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,16 +453,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -821,100 +803,16 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>17.614961496149618</v>
+        <v>15.841859255610379</v>
       </c>
       <c r="C26">
-        <v>46.683006535947726</v>
+        <v>53.306510489336446</v>
       </c>
       <c r="D26">
-        <v>13.770006249829976</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>13.957186544342505</v>
-      </c>
-      <c r="C27">
-        <v>64.922839506172821</v>
-      </c>
-      <c r="D27">
-        <v>11.557255445953455</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28">
-        <v>15.917211328976038</v>
-      </c>
-      <c r="C28">
-        <v>56.515151515151516</v>
-      </c>
-      <c r="D28">
-        <v>9.3708461290691716</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>16.879818594104307</v>
-      </c>
-      <c r="C29">
-        <v>72.738095238095241</v>
-      </c>
-      <c r="D29">
-        <v>10.234497133924256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30">
-        <v>15.620958751393532</v>
-      </c>
-      <c r="C30">
-        <v>43.235294117647058</v>
-      </c>
-      <c r="D30">
-        <v>10.255623100304005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31">
-        <v>15.400313971742543</v>
-      </c>
-      <c r="C31">
-        <v>44.915966386554608</v>
-      </c>
-      <c r="D31">
-        <v>9.2859789319946362</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>15.502564102564106</v>
-      </c>
-      <c r="C32">
-        <v>44.135220125786162</v>
-      </c>
-      <c r="D32">
-        <v>9.7572736188293874</v>
+        <v>10.604497229986412</v>
       </c>
     </row>
   </sheetData>
@@ -927,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21EFAB5C-A166-4816-B0CC-746518748656}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,43 +847,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
       <c r="K1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1933,7 +1831,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>0.84380130389527785</v>
@@ -1974,7 +1872,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1">
         <v>1.35</v>
@@ -2015,7 +1913,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1">
         <v>2.0499999999999998</v>
@@ -2056,7 +1954,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1">
         <v>1.51</v>
@@ -2097,7 +1995,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B29" s="1">
         <v>2.38</v>
@@ -2138,7 +2036,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1">
         <v>2.0439999999999996</v>
@@ -2179,7 +2077,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1">
         <v>3.3748384173669468</v>
@@ -2220,7 +2118,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B32" s="1">
         <v>1.4781107935728699</v>

</xml_diff>